<commit_message>
Update Code in UI-Version_01
</commit_message>
<xml_diff>
--- a/UI_001/XL/Page_1.xlsx
+++ b/UI_001/XL/Page_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sketch_1\Git\UI_1\UI_001\XL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{012C3406-AB23-4D61-AB8C-26F445BE8B2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58B43246-939A-4B31-B01A-2C575E5C8D4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{5EC3F4DB-EF81-46FB-9431-99FD1A794678}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="32">
   <si>
     <t>S.No</t>
   </si>
@@ -115,19 +115,41 @@
   </si>
   <si>
     <t>LoginButton</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>https://opensource-demo.orangehrmlive.com/</t>
+  </si>
+  <si>
+    <t>Add_Button</t>
+  </si>
+  <si>
+    <t>UserRoleSelection</t>
+  </si>
+  <si>
+    <t>Dropdown</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF2A00FF"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -150,8 +172,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -466,18 +491,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEC2C384-F860-427A-A8E8-D7F2F2161104}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="31.54296875" customWidth="1"/>
     <col min="3" max="3" width="23.08984375" customWidth="1"/>
-    <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="14.7265625" customWidth="1"/>
+    <col min="4" max="4" width="51.54296875" customWidth="1"/>
+    <col min="5" max="5" width="17.54296875" customWidth="1"/>
     <col min="6" max="6" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -531,8 +556,8 @@
       <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
-        <v>6</v>
+      <c r="D3" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="E3" t="s">
         <v>6</v>
@@ -658,6 +683,48 @@
         <v>6</v>
       </c>
       <c r="F9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Code Version 2
</commit_message>
<xml_diff>
--- a/UI_001/XL/Page_1.xlsx
+++ b/UI_001/XL/Page_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sketch_1\Git\UI_1\UI_001\XL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0FC2D73-FAF4-402D-98BC-7AEBB09C32F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7376E94-69C2-47BF-A421-0D953429B203}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{5EC3F4DB-EF81-46FB-9431-99FD1A794678}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="40">
   <si>
     <t>S.No</t>
   </si>
@@ -108,9 +108,6 @@
     <t>ScrollUpHOME</t>
   </si>
   <si>
-    <t>Quit</t>
-  </si>
-  <si>
     <t>NewTab</t>
   </si>
   <si>
@@ -144,7 +141,19 @@
     <t>https://ps.uci.edu/~franklin/doc/file_upload.html</t>
   </si>
   <si>
-    <t>Edge</t>
+    <t>Chrome</t>
+  </si>
+  <si>
+    <t>Close</t>
+  </si>
+  <si>
+    <t>TryLogout</t>
+  </si>
+  <si>
+    <t>MouseClick</t>
+  </si>
+  <si>
+    <t>Logout</t>
   </si>
 </sst>
 </file>
@@ -188,7 +197,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -211,11 +220,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -228,6 +248,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -544,8 +565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEC2C384-F860-427A-A8E8-D7F2F2161104}">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -583,10 +604,10 @@
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>5</v>
@@ -729,7 +750,7 @@
         <v>5</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>6</v>
@@ -787,7 +808,7 @@
       <c r="A14" s="2"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>5</v>
@@ -803,10 +824,10 @@
       <c r="A15" s="2"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>5</v>
@@ -822,7 +843,7 @@
         <v>8</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>5</v>
@@ -841,17 +862,17 @@
         <v>5</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="2"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>5</v>
@@ -860,17 +881,17 @@
         <v>5</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="2"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>30</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>31</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>5</v>
@@ -883,10 +904,10 @@
       <c r="A20" s="2"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>5</v>
@@ -899,10 +920,10 @@
       <c r="A21" s="2"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" s="5" t="s">
         <v>30</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>31</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>5</v>
@@ -914,14 +935,34 @@
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="2"/>
       <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
+      <c r="C22" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="2"/>
       <c r="B23" s="3"/>
+      <c r="C23" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="2"/>
@@ -959,7 +1000,7 @@
       <c r="A28" s="2"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>5</v>
@@ -968,10 +1009,15 @@
         <v>5</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2" xr:uid="{4DC76DBA-D34A-4C3F-878A-78FD8CA0460C}">
+      <formula1>$H$2:$H$4</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>